<commit_message>
fix: reformulando sprint backlog
</commit_message>
<xml_diff>
--- a/BackLog Produto/BACKLOG_SPRINTS_DAILY_RETROSPECTIVA.xlsx
+++ b/BackLog Produto/BACKLOG_SPRINTS_DAILY_RETROSPECTIVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erione Technologies\Pim-Terceiro-Semestre-1\BackLog Produto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E0F782-911D-4DC6-953A-A30407A853AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758A00CB-A76A-4F3D-9313-6654BE00D6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{382B0824-085F-46F6-8F9B-52819645303C}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{382B0824-085F-46F6-8F9B-52819645303C}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="212">
   <si>
     <t>PLANEJAMENTO</t>
   </si>
@@ -437,12 +437,6 @@
     <t>TAREFA(S)</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>Todos</t>
-  </si>
-  <si>
     <t>Dev Team</t>
   </si>
   <si>
@@ -473,9 +467,6 @@
     <t>Mateus ; Fábio ; Gabriel</t>
   </si>
   <si>
-    <t>T4</t>
-  </si>
-  <si>
     <t>Arieli; Bia; Luana</t>
   </si>
   <si>
@@ -503,9 +494,6 @@
     <t>Introdução</t>
   </si>
   <si>
-    <t>T8</t>
-  </si>
-  <si>
     <t xml:space="preserve">BAIXA </t>
   </si>
   <si>
@@ -557,13 +545,7 @@
     <t>SPRINT 05</t>
   </si>
   <si>
-    <t>T9</t>
-  </si>
-  <si>
     <t>Gabriel ; Fábio ; Mateus</t>
-  </si>
-  <si>
-    <t>T10</t>
   </si>
   <si>
     <t>Luana; Beatriz ; Arieli</t>
@@ -664,39 +646,6 @@
   </si>
   <si>
     <t>T25- A introdução deve apresentar o tema de modo contextualizado, de forma que fique claro ao leitor qual o objetivo do projeto. É preciso explicitar claramente o objetivo do trabalho e a delimitação do estudo. Pensem que seus leitores precisam entender o foco de seu trabalho logo ao ler o resumo e a introdução.</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>T13 ; T14 ; T15</t>
-  </si>
-  <si>
-    <t>T11 ; T12</t>
-  </si>
-  <si>
-    <t>T16 ; T17</t>
-  </si>
-  <si>
-    <t>T25</t>
-  </si>
-  <si>
-    <t>T22</t>
-  </si>
-  <si>
-    <t>T18</t>
   </si>
   <si>
     <t>Gabriel; Arieli; Mateus</t>
@@ -862,9 +811,6 @@
     <t>06-05-24 | Segunda-Feira</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
     <t>atividade 1</t>
   </si>
   <si>
@@ -926,6 +872,55 @@
   </si>
   <si>
     <t>Gráfico de Burndown (em horas) SPRINT 6</t>
+  </si>
+  <si>
+    <t>T1- pesquisa do que são fazendas urbanas, seus tipos, e relatar um breve histórico no Brasil e no mundo</t>
+  </si>
+  <si>
+    <t>T2- Descrever o que significa segurança alimentar e banco de alimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T3- Explorar os princípios da ODS (Objetivos de Desenvolvimento Sustentável). Explicar o que é ESG (em português meio ambiente, social e governança corporativa) e seu relacionamento com os princípios da ODS. </t>
+  </si>
+  <si>
+    <t>T4- Descrever os objetivos da COP30 (30ª Conferência da ONU sobre Mudanças Climáticas) e como o Brasil está envolvido nesse tema.</t>
+  </si>
+  <si>
+    <t>Luana ; Gabriel</t>
+  </si>
+  <si>
+    <t>Mateus ; Bia</t>
+  </si>
+  <si>
+    <t>Arieli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T5- Descrever os requisitos dos usuários e os requisitos do sistema. </t>
+  </si>
+  <si>
+    <t>T6- Classificar cada requisito (tanto os de usuários quanto os de sistema) como requisito funcional ou não funcional.</t>
+  </si>
+  <si>
+    <t>T7-  Especificar o tipo de cada requisito não funcional levantado (usabilidade, desempenho, capacidade etc.)</t>
+  </si>
+  <si>
+    <t>Mateus ; Beatriz</t>
+  </si>
+  <si>
+    <t>Arieli ; Gabriel</t>
+  </si>
+  <si>
+    <t>Fábio ; Luana</t>
+  </si>
+  <si>
+    <t>T14- Demonstrar o comportamento dos casos de uso por meio do diagrama de sequência.
+ T15- Elaborar o diagrama de implantação (definir quantos servidores, banco de dados, estrutura utilizada para o sistema e como instalar o sistema).</t>
+  </si>
+  <si>
+    <t>T9- Definir e justificar o ciclo de vida de desenvolvimento de software</t>
+  </si>
+  <si>
+    <t>Reformular sprint backlog com as tarefas do backlog.</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -2123,6 +2118,16 @@
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8931,8 +8936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21C7278-4439-4CF1-82AD-0D14D81CCEDD}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8978,7 +8983,7 @@
       <c r="I4" s="119"/>
       <c r="J4" s="120"/>
       <c r="L4" s="117" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="M4" s="117"/>
       <c r="N4" s="117"/>
@@ -8996,7 +9001,7 @@
     </row>
     <row r="6" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="82" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="J6" s="21"/>
       <c r="L6" s="117"/>
@@ -9007,7 +9012,7 @@
     </row>
     <row r="7" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="83" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="J7" s="21"/>
       <c r="L7" s="117"/>
@@ -9018,7 +9023,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B8" s="84" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="J8" s="21"/>
     </row>
@@ -9064,7 +9069,7 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="63" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>7</v>
@@ -9086,7 +9091,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="12" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>7</v>
@@ -9108,7 +9113,7 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>6</v>
@@ -9130,7 +9135,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>6</v>
@@ -9152,7 +9157,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>6</v>
@@ -9174,7 +9179,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>6</v>
@@ -9196,7 +9201,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>7</v>
@@ -9218,7 +9223,7 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>7</v>
@@ -9240,7 +9245,7 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>7</v>
@@ -9261,7 +9266,7 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="12" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>6</v>
@@ -9282,7 +9287,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="12" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>6</v>
@@ -9303,7 +9308,7 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="12" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="7">
@@ -9323,7 +9328,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>7</v>
@@ -9344,7 +9349,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>43</v>
@@ -9365,7 +9370,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>38</v>
@@ -9380,14 +9385,14 @@
     <row r="26" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="72"/>
       <c r="B26" s="37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>5</v>
@@ -9401,14 +9406,14 @@
     </row>
     <row r="27" spans="1:10" ht="175.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="77" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="71" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>5</v>
@@ -9422,14 +9427,14 @@
     </row>
     <row r="28" spans="1:10" ht="198.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="35" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="71" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>5</v>
@@ -9443,14 +9448,14 @@
     </row>
     <row r="29" spans="1:10" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="77" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="71" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>5</v>
@@ -9464,14 +9469,14 @@
     </row>
     <row r="30" spans="1:10" ht="149" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="4" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>5</v>
@@ -9485,14 +9490,14 @@
     </row>
     <row r="31" spans="1:10" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="78" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C31" s="79" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D31" s="80"/>
       <c r="E31" s="79" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F31" s="81" t="s">
         <v>5</v>
@@ -9511,7 +9516,7 @@
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="G33" s="130" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H33" s="131"/>
       <c r="I33" s="131"/>
@@ -9523,10 +9528,10 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I34" s="24"/>
       <c r="J34" s="24"/>
@@ -9537,11 +9542,11 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H35" s="28"/>
       <c r="I35" s="124" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J35" s="125"/>
     </row>
@@ -9551,7 +9556,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H36" s="28"/>
       <c r="I36" s="126"/>
@@ -9563,7 +9568,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H37" s="28"/>
       <c r="I37" s="126"/>
@@ -9575,7 +9580,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H38" s="28"/>
       <c r="I38" s="126"/>
@@ -9587,7 +9592,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H39" s="28"/>
       <c r="I39" s="126"/>
@@ -9599,7 +9604,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H40" s="28"/>
       <c r="I40" s="128"/>
@@ -9681,16 +9686,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E39882E-15E1-49D7-8705-F56E6D1328C9}">
-  <dimension ref="C1:K71"/>
+  <dimension ref="C1:K83"/>
   <sheetViews>
     <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.08984375" customWidth="1"/>
     <col min="5" max="5" width="12.26953125" customWidth="1"/>
     <col min="6" max="6" width="21.90625" customWidth="1"/>
     <col min="7" max="7" width="22.6328125" customWidth="1"/>
@@ -9706,7 +9711,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="H2" s="130" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="131"/>
       <c r="J2" s="131"/>
@@ -9718,10 +9723,10 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
@@ -9732,11 +9737,11 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="124" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K4" s="125"/>
     </row>
@@ -9746,7 +9751,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="126"/>
@@ -9758,7 +9763,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="126"/>
@@ -9770,7 +9775,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="126"/>
@@ -9782,7 +9787,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="126"/>
@@ -9794,7 +9799,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="128"/>
@@ -9905,19 +9910,19 @@
         <v>11</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J22" s="20" t="s">
         <v>4</v>
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="3:11" ht="16" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:11" ht="87.5" x14ac:dyDescent="0.4">
       <c r="C23" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>63</v>
+      <c r="D23" s="148" t="s">
+        <v>196</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>7</v>
@@ -9926,7 +9931,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>64</v>
+        <v>200</v>
       </c>
       <c r="H23" s="30">
         <v>3</v>
@@ -9935,13 +9940,13 @@
         <v>45383</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" ht="16" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" ht="58.5" x14ac:dyDescent="0.4">
       <c r="C24" s="35"/>
-      <c r="D24" s="2" t="s">
-        <v>136</v>
+      <c r="D24" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>7</v>
@@ -9950,7 +9955,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H24" s="16">
         <v>3</v>
@@ -9959,13 +9964,13 @@
         <v>45383</v>
       </c>
       <c r="J24" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" ht="16" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="189" x14ac:dyDescent="0.4">
       <c r="C25" s="35"/>
-      <c r="D25" s="2" t="s">
-        <v>137</v>
+      <c r="D25" s="4" t="s">
+        <v>198</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>7</v>
@@ -9974,7 +9979,7 @@
         <v>5</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>64</v>
+        <v>201</v>
       </c>
       <c r="H25" s="16">
         <v>3</v>
@@ -9983,13 +9988,13 @@
         <v>45383</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" ht="16" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" ht="131" x14ac:dyDescent="0.4">
       <c r="C26" s="35"/>
-      <c r="D26" s="2" t="s">
-        <v>75</v>
+      <c r="D26" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>7</v>
@@ -9998,7 +10003,7 @@
         <v>5</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
       <c r="H26" s="16">
         <v>3</v>
@@ -10007,7 +10012,7 @@
         <v>45383</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10057,19 +10062,19 @@
         <v>11</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J32" s="20" t="s">
         <v>4</v>
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="3:10" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:10" ht="73" x14ac:dyDescent="0.4">
       <c r="C33" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>138</v>
+      <c r="D33" s="148" t="s">
+        <v>203</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>7</v>
@@ -10078,7 +10083,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="H33" s="30">
         <v>6</v>
@@ -10087,13 +10092,13 @@
         <v>45390</v>
       </c>
       <c r="J33" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="16" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="102" x14ac:dyDescent="0.4">
       <c r="C34" s="35"/>
-      <c r="D34" s="17" t="s">
-        <v>139</v>
+      <c r="D34" s="148" t="s">
+        <v>204</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>7</v>
@@ -10102,7 +10107,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="H34" s="30">
         <v>6</v>
@@ -10111,13 +10116,13 @@
         <v>45390</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="16" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="102" x14ac:dyDescent="0.4">
       <c r="C35" s="35"/>
-      <c r="D35" s="17" t="s">
-        <v>140</v>
+      <c r="D35" s="148" t="s">
+        <v>205</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>7</v>
@@ -10126,7 +10131,7 @@
         <v>5</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>64</v>
+        <v>208</v>
       </c>
       <c r="H35" s="30">
         <v>6</v>
@@ -10135,7 +10140,7 @@
         <v>45390</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10151,7 +10156,7 @@
     <row r="38" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="39" spans="3:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C39" s="133" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D39" s="134"/>
       <c r="E39" s="134"/>
@@ -10185,18 +10190,18 @@
         <v>11</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J41" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="3:10" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:10" ht="339.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C42" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>141</v>
+      <c r="D42" s="148" t="s">
+        <v>120</v>
       </c>
       <c r="E42" s="44" t="s">
         <v>7</v>
@@ -10205,7 +10210,7 @@
         <v>8</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H42" s="45">
         <v>4</v>
@@ -10214,417 +10219,517 @@
         <v>45397</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="37"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="31"/>
+    </row>
+    <row r="44" spans="3:10" ht="230" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="10" t="s">
+      <c r="D44" s="149" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="48">
+      <c r="F44" s="48">
         <v>5</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H43" s="7">
+      <c r="G44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H44" s="7">
         <v>5</v>
       </c>
-      <c r="I43" s="38">
+      <c r="I44" s="38">
         <v>45397</v>
       </c>
-      <c r="J43" s="39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="36"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="23"/>
-    </row>
-    <row r="46" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="47" spans="3:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C47" s="133" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="134"/>
-      <c r="E47" s="134"/>
-      <c r="F47" s="134"/>
-      <c r="G47" s="134"/>
-      <c r="H47" s="134"/>
-      <c r="I47" s="134"/>
-      <c r="J47" s="135"/>
-    </row>
-    <row r="48" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C48" s="32"/>
-      <c r="J48" s="21"/>
+      <c r="J44" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C45" s="36"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="23"/>
+    </row>
+    <row r="47" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="48" spans="3:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C48" s="133" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="134"/>
+      <c r="E48" s="134"/>
+      <c r="F48" s="134"/>
+      <c r="G48" s="134"/>
+      <c r="H48" s="134"/>
+      <c r="I48" s="134"/>
+      <c r="J48" s="135"/>
     </row>
     <row r="49" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="32"/>
+      <c r="J49" s="21"/>
+    </row>
+    <row r="50" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="E50" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="F50" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="19" t="s">
+      <c r="G50" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="19" t="s">
+      <c r="H50" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I49" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="J49" s="20" t="s">
+      <c r="I50" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J50" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="16" x14ac:dyDescent="0.35">
-      <c r="C50" s="43" t="s">
+    <row r="51" spans="3:10" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C51" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="E50" s="44" t="s">
+      <c r="D51" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="E51" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="47">
+      <c r="F51" s="47">
         <v>4</v>
       </c>
-      <c r="G50" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H50" s="30">
+      <c r="G51" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H51" s="30">
         <v>2</v>
       </c>
-      <c r="I50" s="29">
+      <c r="I51" s="29">
         <v>45404</v>
       </c>
-      <c r="J50" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C51" s="37" t="s">
+      <c r="J51" s="34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C52" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E51" s="10" t="s">
+      <c r="D52" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="48">
+      <c r="F52" s="48">
         <v>9</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H51" s="7">
+      <c r="G52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H52" s="7">
         <v>5</v>
-      </c>
-      <c r="I51" s="38">
-        <v>45404</v>
-      </c>
-      <c r="J51" s="41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10" ht="16" x14ac:dyDescent="0.35">
-      <c r="C52" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="F52" s="48">
-        <v>2</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H52" s="7">
-        <v>7</v>
       </c>
       <c r="I52" s="38">
         <v>45404</v>
       </c>
       <c r="J52" s="41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C53" s="36"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="23"/>
-    </row>
-    <row r="55" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="56" spans="3:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C56" s="133" t="s">
-        <v>102</v>
-      </c>
-      <c r="D56" s="134"/>
-      <c r="E56" s="134"/>
-      <c r="F56" s="134"/>
-      <c r="G56" s="134"/>
-      <c r="H56" s="134"/>
-      <c r="I56" s="134"/>
-      <c r="J56" s="135"/>
-    </row>
-    <row r="57" spans="3:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C57" s="32"/>
-      <c r="J57" s="21"/>
-    </row>
-    <row r="58" spans="3:10" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C58" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" ht="200" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C53" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" s="48">
+        <v>2</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H53" s="7">
+        <v>7</v>
+      </c>
+      <c r="I53" s="38">
+        <v>45404</v>
+      </c>
+      <c r="J53" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C54" s="36"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="23"/>
+    </row>
+    <row r="56" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="3:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C57" s="133" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="134"/>
+      <c r="E57" s="134"/>
+      <c r="F57" s="134"/>
+      <c r="G57" s="134"/>
+      <c r="H57" s="134"/>
+      <c r="I57" s="134"/>
+      <c r="J57" s="135"/>
+    </row>
+    <row r="58" spans="3:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C58" s="32"/>
+      <c r="J58" s="21"/>
+    </row>
+    <row r="59" spans="3:10" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C59" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D59" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E59" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F59" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G59" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H58" s="19" t="s">
+      <c r="H59" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I58" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="J58" s="20" t="s">
+      <c r="I59" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J59" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="3:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E59" s="44" t="s">
+    <row r="60" spans="3:10" ht="164" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C60" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="148" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F59" s="45">
+      <c r="F60" s="45">
         <v>13</v>
       </c>
-      <c r="G59" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H59" s="45">
+      <c r="G60" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H60" s="45">
         <v>7</v>
       </c>
-      <c r="I59" s="29">
+      <c r="I60" s="29">
         <v>45411</v>
       </c>
-      <c r="J59" s="41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C60" s="37" t="s">
+      <c r="J60" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C61" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E60" s="10" t="s">
+      <c r="D61" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F61" s="7">
         <v>9</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H60" s="7">
+      <c r="G61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H61" s="7">
         <v>6.5</v>
       </c>
-      <c r="I60" s="38">
+      <c r="I61" s="38">
         <v>45411</v>
       </c>
-      <c r="J60" s="41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C61" s="36"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="23"/>
-    </row>
-    <row r="64" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="65" spans="3:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C65" s="133" t="s">
-        <v>167</v>
-      </c>
-      <c r="D65" s="134"/>
-      <c r="E65" s="134"/>
-      <c r="F65" s="134"/>
-      <c r="G65" s="134"/>
-      <c r="H65" s="134"/>
-      <c r="I65" s="134"/>
-      <c r="J65" s="135"/>
-    </row>
-    <row r="66" spans="3:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C66" s="32"/>
-      <c r="J66" s="21"/>
-    </row>
-    <row r="67" spans="3:10" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C67" s="18" t="s">
+      <c r="J61" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C62" s="36"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="23"/>
+    </row>
+    <row r="65" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="66" spans="3:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C66" s="133" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="134"/>
+      <c r="E66" s="134"/>
+      <c r="F66" s="134"/>
+      <c r="G66" s="134"/>
+      <c r="H66" s="134"/>
+      <c r="I66" s="134"/>
+      <c r="J66" s="135"/>
+    </row>
+    <row r="67" spans="3:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C67" s="32"/>
+      <c r="J67" s="21"/>
+    </row>
+    <row r="68" spans="3:10" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C68" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D68" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E68" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F67" s="19" t="s">
+      <c r="F68" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G68" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H67" s="19" t="s">
+      <c r="H68" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I67" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="J67" s="20" t="s">
+      <c r="I68" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J68" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="3:10" ht="117.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C68" s="43" t="s">
+    <row r="69" spans="3:10" ht="164" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C69" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E68" s="44" t="s">
+      <c r="D69" s="148" t="s">
+        <v>122</v>
+      </c>
+      <c r="E69" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="45">
+      <c r="F69" s="45">
         <v>10</v>
       </c>
-      <c r="G68" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="H68" s="45">
+      <c r="G69" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="H69" s="45">
         <v>7</v>
       </c>
-      <c r="I68" s="29">
+      <c r="I69" s="29">
         <v>45418</v>
       </c>
-      <c r="J68" s="34" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="3:10" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C69" s="69" t="s">
+      <c r="J69" s="34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C70" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E69" s="9" t="s">
+      <c r="D70" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F70" s="7">
         <v>7</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H69" s="7">
+      <c r="G70" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H70" s="7">
         <v>3</v>
-      </c>
-      <c r="I69" s="38">
-        <v>45418</v>
-      </c>
-      <c r="J69" s="41" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="70" spans="3:10" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C70" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" s="7">
-        <v>9</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H70" s="7">
-        <v>10</v>
       </c>
       <c r="I70" s="38">
         <v>45418</v>
       </c>
       <c r="J70" s="41" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="78"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="80"/>
-      <c r="F71" s="80"/>
-      <c r="G71" s="80"/>
-      <c r="H71" s="80"/>
-      <c r="I71" s="80"/>
-      <c r="J71" s="61"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C71" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="7">
+        <v>9</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H71" s="7">
+        <v>10</v>
+      </c>
+      <c r="I71" s="38">
+        <v>45418</v>
+      </c>
+      <c r="J71" s="41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C72" s="78"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="80"/>
+      <c r="J72" s="61"/>
+    </row>
+    <row r="76" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="3:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C77" s="133" t="s">
+        <v>150</v>
+      </c>
+      <c r="D77" s="134"/>
+      <c r="E77" s="134"/>
+      <c r="F77" s="134"/>
+      <c r="G77" s="134"/>
+      <c r="H77" s="134"/>
+      <c r="I77" s="134"/>
+      <c r="J77" s="135"/>
+    </row>
+    <row r="78" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C78" s="32"/>
+      <c r="D78" s="151"/>
+      <c r="E78" s="151"/>
+      <c r="F78" s="151"/>
+      <c r="G78" s="151"/>
+      <c r="H78" s="151"/>
+      <c r="I78" s="151"/>
+      <c r="J78" s="21"/>
+    </row>
+    <row r="79" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C79" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H79" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I79" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J79" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C80" s="32"/>
+      <c r="D80" s="151"/>
+      <c r="E80" s="151"/>
+      <c r="F80" s="151"/>
+      <c r="G80" s="151"/>
+      <c r="H80" s="151"/>
+      <c r="I80" s="151"/>
+      <c r="J80" s="21"/>
+    </row>
+    <row r="81" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C81" s="32"/>
+      <c r="D81" s="151"/>
+      <c r="E81" s="151"/>
+      <c r="F81" s="151"/>
+      <c r="G81" s="151"/>
+      <c r="H81" s="151"/>
+      <c r="I81" s="151"/>
+      <c r="J81" s="21"/>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C82" s="32"/>
+      <c r="D82" s="151"/>
+      <c r="E82" s="151"/>
+      <c r="F82" s="151"/>
+      <c r="G82" s="151"/>
+      <c r="H82" s="151"/>
+      <c r="I82" s="151"/>
+      <c r="J82" s="21"/>
+    </row>
+    <row r="83" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C83" s="36"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="22"/>
+      <c r="J83" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C56:J56"/>
-    <mergeCell ref="C65:J65"/>
+  <mergeCells count="10">
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="C66:J66"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="J4:K9"/>
     <mergeCell ref="C15:J15"/>
@@ -10640,7 +10745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53D959B-E411-475F-8D2F-46A6BAEF8854}">
   <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="94" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="94" workbookViewId="0">
       <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
@@ -10653,7 +10758,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="133" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B1" s="134"/>
       <c r="C1" s="135"/>
@@ -10699,7 +10804,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -10721,7 +10826,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -10748,7 +10853,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -10759,7 +10864,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -10770,7 +10875,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -10781,7 +10886,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -10792,7 +10897,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -10803,7 +10908,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -10819,7 +10924,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -10830,7 +10935,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -10841,7 +10946,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -10849,10 +10954,10 @@
         <v>45407</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -10863,7 +10968,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -10874,7 +10979,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -10890,7 +10995,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -10901,7 +11006,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="54" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -10912,7 +11017,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -10920,10 +11025,10 @@
         <v>45408</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -10934,7 +11039,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10945,7 +11050,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -10961,7 +11066,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -10972,7 +11077,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -10983,7 +11088,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -10991,10 +11096,10 @@
         <v>45409</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -11005,7 +11110,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11016,7 +11121,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="61" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -11032,7 +11137,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -11043,7 +11148,7 @@
         <v>19</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -11054,7 +11159,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -11062,10 +11167,10 @@
         <v>45410</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -11076,7 +11181,7 @@
         <v>21</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11087,7 +11192,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="61" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -11103,7 +11208,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -11114,7 +11219,7 @@
         <v>19</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -11125,7 +11230,7 @@
         <v>22</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -11133,10 +11238,10 @@
         <v>45411</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -11147,7 +11252,7 @@
         <v>21</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11158,13 +11263,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="61" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="54" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A54" s="142" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B54" s="143"/>
       <c r="C54" s="144"/>
@@ -11177,7 +11282,7 @@
         <v>17</v>
       </c>
       <c r="C55" s="54" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -11188,7 +11293,7 @@
         <v>19</v>
       </c>
       <c r="C56" s="54" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -11199,7 +11304,7 @@
         <v>22</v>
       </c>
       <c r="C57" s="54" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -11207,10 +11312,10 @@
         <v>45412</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C58" s="54" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -11221,7 +11326,7 @@
         <v>21</v>
       </c>
       <c r="C59" s="54" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11232,7 +11337,7 @@
         <v>25</v>
       </c>
       <c r="C60" s="61" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -11248,7 +11353,7 @@
         <v>17</v>
       </c>
       <c r="C62" s="54" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -11259,7 +11364,7 @@
         <v>19</v>
       </c>
       <c r="C63" s="54" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -11270,7 +11375,7 @@
         <v>22</v>
       </c>
       <c r="C64" s="54" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -11278,10 +11383,10 @@
         <v>45413</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C65" s="54" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -11292,7 +11397,7 @@
         <v>21</v>
       </c>
       <c r="C66" s="54" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11303,7 +11408,7 @@
         <v>25</v>
       </c>
       <c r="C67" s="54" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -11319,7 +11424,7 @@
         <v>17</v>
       </c>
       <c r="C69" s="54" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -11330,7 +11435,7 @@
         <v>19</v>
       </c>
       <c r="C70" s="54" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -11341,7 +11446,7 @@
         <v>22</v>
       </c>
       <c r="C71" s="54" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -11349,10 +11454,10 @@
         <v>45414</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C72" s="54" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -11363,7 +11468,7 @@
         <v>21</v>
       </c>
       <c r="C73" s="54" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11374,7 +11479,7 @@
         <v>25</v>
       </c>
       <c r="C74" s="61" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -11390,7 +11495,7 @@
         <v>17</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -11401,7 +11506,7 @@
         <v>19</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -11412,7 +11517,7 @@
         <v>22</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -11420,10 +11525,10 @@
         <v>45415</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -11434,7 +11539,7 @@
         <v>21</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11445,7 +11550,7 @@
         <v>25</v>
       </c>
       <c r="C81" s="54" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11461,7 +11566,7 @@
         <v>17</v>
       </c>
       <c r="C83" s="96" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11472,7 +11577,7 @@
         <v>19</v>
       </c>
       <c r="C84" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11483,7 +11588,7 @@
         <v>22</v>
       </c>
       <c r="C85" s="54" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11491,10 +11596,10 @@
         <v>45416</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C86" s="54" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11505,7 +11610,7 @@
         <v>21</v>
       </c>
       <c r="C87" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11516,7 +11621,7 @@
         <v>25</v>
       </c>
       <c r="C88" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11532,7 +11637,7 @@
         <v>17</v>
       </c>
       <c r="C90" s="96" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11543,7 +11648,7 @@
         <v>19</v>
       </c>
       <c r="C91" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11554,7 +11659,7 @@
         <v>22</v>
       </c>
       <c r="C92" s="54" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11562,10 +11667,10 @@
         <v>45417</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C93" s="54" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11576,7 +11681,7 @@
         <v>21</v>
       </c>
       <c r="C94" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -11587,7 +11692,7 @@
         <v>25</v>
       </c>
       <c r="C95" s="54" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -11603,7 +11708,7 @@
         <v>17</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -11614,7 +11719,7 @@
         <v>19</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -11625,7 +11730,7 @@
         <v>22</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -11633,10 +11738,10 @@
         <v>45418</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -11647,7 +11752,7 @@
         <v>21</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11658,7 +11763,7 @@
         <v>25</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -11698,7 +11803,7 @@
         <v>45419</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C107" s="54"/>
     </row>
@@ -11736,7 +11841,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11747,7 +11852,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="145" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B1" s="146"/>
       <c r="C1" s="65"/>
@@ -11763,42 +11868,42 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="42" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="67" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B6" s="86" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="54.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="67" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -11813,7 +11918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E69F5A-B02F-42AF-8116-2B76A69569A0}">
   <dimension ref="A5:R149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
@@ -11828,13 +11933,13 @@
   <sheetData>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="16" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
@@ -11916,7 +12021,7 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="16" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C13" s="16">
         <v>0</v>
@@ -11927,13 +12032,13 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
@@ -12015,7 +12120,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B34" s="16" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C34" s="16">
         <v>0</v>
@@ -12111,7 +12216,7 @@
     </row>
     <row r="47" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="147" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B47" s="147"/>
       <c r="C47" s="147"/>
@@ -12254,34 +12359,34 @@
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="101"/>
       <c r="B54" s="106" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="C54" s="107" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D54" s="108" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="E54" s="108" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="F54" s="108" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="G54" s="108" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="H54" s="108" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="I54" s="108" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="J54" s="108" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="K54" s="109" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="L54" s="101"/>
       <c r="M54" s="101"/>
@@ -12294,7 +12399,7 @@
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="101"/>
       <c r="B55" s="102" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="C55" s="103">
         <v>20</v>
@@ -12328,7 +12433,7 @@
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="101"/>
       <c r="B56" s="102" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="C56" s="104">
         <v>10</v>
@@ -12356,7 +12461,7 @@
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="101"/>
       <c r="B57" s="102" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C57" s="104">
         <v>15</v>
@@ -12388,7 +12493,7 @@
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="101"/>
       <c r="B58" s="102" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C58" s="104">
         <v>10</v>
@@ -12418,7 +12523,7 @@
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="101"/>
       <c r="B59" s="102" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C59" s="104">
         <v>8</v>
@@ -12450,7 +12555,7 @@
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="101"/>
       <c r="B60" s="102" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C60" s="104">
         <v>12</v>
@@ -12484,7 +12589,7 @@
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="101"/>
       <c r="B61" s="102" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="C61" s="104">
         <v>15</v>
@@ -12518,7 +12623,7 @@
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="101"/>
       <c r="B62" s="102" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C62" s="104">
         <v>8</v>
@@ -12550,7 +12655,7 @@
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="101"/>
       <c r="B63" s="102" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C63" s="104">
         <v>12</v>
@@ -12580,7 +12685,7 @@
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="101"/>
       <c r="B64" s="102" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C64" s="104">
         <v>10</v>
@@ -12610,58 +12715,44 @@
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="101"/>
       <c r="B65" s="110" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="C65" s="111">
         <f>SUM(C55:C64)</f>
         <v>120</v>
       </c>
       <c r="D65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
+        <f t="shared" ref="D65:K65" si="0">IF(SUM($D$55:$D$64)&gt;0,
 C$65-SUM(D$55:D$64),
 NA())</f>
         <v>108</v>
       </c>
       <c r="E65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-D$65-SUM(E$55:E$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="F65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-E$65-SUM(F$55:F$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="G65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-F$65-SUM(G$55:G$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="H65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-G$65-SUM(H$55:H$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="I65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-H$65-SUM(I$55:I$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="J65" s="111">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-I$65-SUM(J$55:J$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="K65" s="112">
-        <f>IF(SUM($D$55:$D$64)&gt;0,
-J$65-SUM(K$55:K$64),
-NA())</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L65" s="101"/>
@@ -12674,41 +12765,41 @@
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="101"/>
       <c r="B66" s="113" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C66" s="114">
         <v>120</v>
       </c>
       <c r="D66" s="114">
-        <f>C$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" ref="D66:K66" si="1">C$66-($C$66/COUNTA($D$54:$K$54))</f>
         <v>105</v>
       </c>
       <c r="E66" s="114">
-        <f>D$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="F66" s="114">
-        <f>E$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="G66" s="114">
-        <f>F$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H66" s="114">
-        <f>G$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="I66" s="114">
-        <f>H$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="J66" s="114">
-        <f>I$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="K66" s="115">
-        <f>J$66-($C$66/COUNTA($D$54:$K$54))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L66" s="101"/>
@@ -12865,13 +12956,13 @@
     </row>
     <row r="106" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C106" s="16" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="3:5" x14ac:dyDescent="0.35">
@@ -12953,7 +13044,7 @@
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C114" s="16" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D114" s="16">
         <v>0</v>
@@ -12964,13 +13055,13 @@
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C124" s="16" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E124" s="16" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.35">
@@ -13052,7 +13143,7 @@
     </row>
     <row r="132" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C132" s="16" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D132" s="16">
         <v>0</v>
@@ -13063,13 +13154,13 @@
     </row>
     <row r="141" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C141" s="16" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="D141" s="16" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E141" s="16" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="142" spans="3:5" x14ac:dyDescent="0.35">
@@ -13151,7 +13242,7 @@
     </row>
     <row r="149" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C149" s="16" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D149" s="16">
         <v>0</v>

</xml_diff>